<commit_message>
ETRM MT & Date
</commit_message>
<xml_diff>
--- a/testData/ExecuteTask/Notification/ETRM/ET_NT_ETRM_CTAfterDays_Test.xlsx
+++ b/testData/ExecuteTask/Notification/ETRM/ET_NT_ETRM_CTAfterDays_Test.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="87">
   <si>
     <t>ModuleName</t>
   </si>
@@ -262,12 +262,34 @@
   </si>
   <si>
     <t xml:space="preserve">ET_ETRM_Notify </t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>30-05-2024</t>
+  </si>
+  <si>
+    <t>30-05-2024 12:07:36 PM</t>
+  </si>
+  <si>
+    <t>ET455</t>
+  </si>
+  <si>
+    <t>30-05-2024 12:13:38 PM</t>
+  </si>
+  <si>
+    <t>ET456</t>
+  </si>
+  <si>
+    <t>ET457</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -622,34 +644,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="17" width="9.1796875" style="1"/>
-    <col min="18" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.1796875" style="1"/>
-    <col min="20" max="20" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="9.1796875" style="1"/>
-    <col min="24" max="24" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="13.26953125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="25.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="11.1796875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.54296875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="14.7265625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="20.0"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="12.54296875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="11.1796875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="16.81640625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="8.81640625"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.08984375"/>
+    <col min="12" max="17" style="1" width="9.1796875"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="11.0"/>
+    <col min="19" max="19" style="1" width="9.1796875"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="23.0"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.0"/>
+    <col min="22" max="23" style="1" width="9.1796875"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="18.81640625"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="20.0"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="16.26953125"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="33.54296875"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="8.81640625"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.81640625"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="20.0"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.0"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="19.81640625"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="12.26953125"/>
+    <col min="34" max="16384" style="1" width="9.1796875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.35">
@@ -784,8 +806,8 @@
       <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>69</v>
+      <c r="K2" t="s" s="1">
+        <v>81</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -793,10 +815,10 @@
       <c r="M2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="N2" t="s" s="1">
+        <v>82</v>
+      </c>
+      <c r="O2" t="s" s="1">
         <v>72</v>
       </c>
       <c r="P2" s="1" t="s">
@@ -847,11 +869,11 @@
       <c r="AF2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AG2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>68</v>
+      <c r="AG2" t="s" s="1">
+        <v>83</v>
+      </c>
+      <c r="AK2" t="s" s="1">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -873,23 +895,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.7265625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.7265625"/>
+    <col min="6" max="6" customWidth="true" width="21.453125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.54296875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.81640625"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.81640625"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="21.7265625"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.453125"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="23.81640625"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="20.0"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.26953125"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="33.54296875"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.81640625"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="19.81640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
@@ -1024,8 +1046,8 @@
       <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s">
-        <v>69</v>
+      <c r="K2" t="s" s="0">
+        <v>81</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -1033,10 +1055,10 @@
       <c r="M2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N2" t="s">
-        <v>70</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="O2" t="s" s="0">
         <v>72</v>
       </c>
       <c r="P2" s="1" t="s">
@@ -1086,8 +1108,8 @@
       <c r="AF2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AG2" t="s">
-        <v>74</v>
+      <c r="AG2" t="s" s="0">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1110,12 +1132,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.7265625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.7265625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.26953125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.81640625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.1796875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
@@ -1250,8 +1272,8 @@
       <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s">
-        <v>69</v>
+      <c r="K2" t="s" s="0">
+        <v>81</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -1259,10 +1281,10 @@
       <c r="M2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N2" t="s">
-        <v>70</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="O2" t="s" s="0">
         <v>72</v>
       </c>
       <c r="P2" s="1" t="s">
@@ -1312,8 +1334,8 @@
       <c r="AF2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AG2" t="s">
-        <v>75</v>
+      <c r="AG2" t="s" s="0">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1335,11 +1357,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.1796875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.7265625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.453125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.1796875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
@@ -1474,8 +1496,8 @@
       <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s">
-        <v>69</v>
+      <c r="K2" t="s" s="0">
+        <v>81</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -1483,10 +1505,10 @@
       <c r="M2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N2" t="s">
-        <v>70</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="O2" t="s" s="0">
         <v>72</v>
       </c>
       <c r="P2" s="1" t="s">
@@ -1536,8 +1558,8 @@
       <c r="AF2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AG2" t="s">
-        <v>75</v>
+      <c r="AG2" t="s" s="0">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>